<commit_message>
new sites to yandex
</commit_message>
<xml_diff>
--- a/res.xlsx
+++ b/res.xlsx
@@ -17,6 +17,32 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+  <si>
+    <t>11.25.2019 14:35:18</t>
+  </si>
+  <si>
+    <t>−6</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>11.25.2019 14:36:44</t>
+  </si>
+  <si>
+    <t>11.25.2019 14:37:01</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -112,7 +138,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A2:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -120,9 +146,70 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.49"/>
+    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="10.49" collapsed="true" outlineLevel="0"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>